<commit_message>
Não mandar essa versao para o onrender
</commit_message>
<xml_diff>
--- a/modelo_os_new.xlsx
+++ b/modelo_os_new.xlsx
@@ -1011,7 +1011,7 @@
         </is>
       </c>
       <c r="B8" s="6" t="n">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="C8" s="7" t="n"/>
       <c r="D8" s="8" t="n"/>
@@ -1023,7 +1023,7 @@
       </c>
       <c r="G8" s="11" t="inlineStr">
         <is>
-          <t>04/07/2023</t>
+          <t>05/07/2023</t>
         </is>
       </c>
       <c r="H8" s="12" t="n"/>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="G9" s="17" t="inlineStr">
         <is>
-          <t>14:54</t>
+          <t>10:50</t>
         </is>
       </c>
       <c r="H9" s="12" t="n"/>
@@ -1114,7 +1114,7 @@
       </c>
       <c r="B12" s="27" t="inlineStr">
         <is>
-          <t>Ponte expedicao ficou presa nas grades da deltec</t>
+          <t xml:space="preserve">Ponte cabine pó com vazamento de óleo </t>
         </is>
       </c>
       <c r="C12" s="28" t="n"/>

</xml_diff>